<commit_message>
added whylogs, great expectations and facets
</commit_message>
<xml_diff>
--- a/tools/tool_comparison.xlsx
+++ b/tools/tool_comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\hedderich\repos\MLOps\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF27F2A0-7A06-4BCC-91B9-EFFE780EE751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D26DFEBA-016B-4812-87C9-4CCA02FE551E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="437">
   <si>
     <t>Name</t>
   </si>
@@ -1313,6 +1313,24 @@
   </si>
   <si>
     <t>https://github.com/online-ml/river</t>
+  </si>
+  <si>
+    <t>https://github.com/whylabs/whylogs</t>
+  </si>
+  <si>
+    <t>whylogs</t>
+  </si>
+  <si>
+    <t>https://github.com/great-expectations/great_expectations</t>
+  </si>
+  <si>
+    <t>Great Expectations</t>
+  </si>
+  <si>
+    <t>https://github.com/PAIR-code/facets</t>
+  </si>
+  <si>
+    <t>facets</t>
   </si>
 </sst>
 </file>
@@ -1680,14 +1698,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y66"/>
+  <dimension ref="A1:Y69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
+    <col min="1" max="1" width="18.84375" customWidth="1"/>
     <col min="2" max="2" width="44.3046875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.4609375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.69140625" bestFit="1" customWidth="1"/>
@@ -6273,6 +6292,30 @@
         <v>430</v>
       </c>
     </row>
+    <row r="67" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A67" t="s">
+        <v>432</v>
+      </c>
+      <c r="B67" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="68" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A68" t="s">
+        <v>434</v>
+      </c>
+      <c r="B68" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="69" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A69" t="s">
+        <v>436</v>
+      </c>
+      <c r="B69" t="s">
+        <v>435</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>